<commit_message>
Added meeting info (BCY)
</commit_message>
<xml_diff>
--- a/ExpensesCalculator.xlsx
+++ b/ExpensesCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\BeverlyPC\Documents\SetsunaFolder\School\CS3992\LEDWaterFountain\public_html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C41956-DDDF-4B96-BCB0-24B5BD176FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC7470F-8066-4D42-BEE2-7C162416F9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16110" windowWidth="29040" windowHeight="16440" xr2:uid="{0D8CD52F-8563-45E9-9F35-2D7721D21F4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{0D8CD52F-8563-45E9-9F35-2D7721D21F4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Item</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Bev</t>
+  </si>
+  <si>
+    <t>solder paste</t>
+  </si>
+  <si>
+    <t>LED strip lights</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBABB7F-8FB9-4334-82A1-0F1C5A07B0CC}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="G22" sqref="G22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -630,26 +636,42 @@
         <v>11.45</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G17">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16">
+        <v>12.82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17">
+        <v>73.959999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21">
         <f>SUM(G2:G15)</f>
         <v>151.88</v>
       </c>
-      <c r="H17">
-        <f>SUM(H2:H15)</f>
-        <v>126.07000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G18" s="2">
-        <f>G17+H17</f>
-        <v>277.95</v>
-      </c>
-      <c r="H18" s="2"/>
+      <c r="H21">
+        <f>SUM(H2:H17)</f>
+        <v>212.85000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="2">
+        <f>G21+H21</f>
+        <v>364.73</v>
+      </c>
+      <c r="H22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pumps Attached, tray finished images (BCY)
</commit_message>
<xml_diff>
--- a/ExpensesCalculator.xlsx
+++ b/ExpensesCalculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\BeverlyPC\Documents\SetsunaFolder\School\CS3992\LEDWaterFountain\public_html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC7470F-8066-4D42-BEE2-7C162416F9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D6D52B-063A-41C5-BC77-EF5421B91061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{0D8CD52F-8563-45E9-9F35-2D7721D21F4F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Item</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>LED strip lights</t>
+  </si>
+  <si>
+    <t>contour tool</t>
+  </si>
+  <si>
+    <t>electronic silicone</t>
   </si>
 </sst>
 </file>
@@ -140,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -148,11 +154,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -160,6 +175,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBABB7F-8FB9-4334-82A1-0F1C5A07B0CC}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22:H22"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -640,6 +657,9 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
+      <c r="C16" s="4">
+        <v>45058</v>
+      </c>
       <c r="H16">
         <v>12.82</v>
       </c>
@@ -652,26 +672,75 @@
         <v>73.959999999999994</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G21">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="4">
+        <v>45035</v>
+      </c>
+      <c r="H18">
+        <v>11.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4">
+        <v>45145</v>
+      </c>
+      <c r="H19">
+        <v>10.67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G23">
         <f>SUM(G2:G15)</f>
         <v>151.88</v>
       </c>
-      <c r="H21">
+      <c r="H23">
         <f>SUM(H2:H17)</f>
         <v>212.85000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G22" s="2">
-        <f>G21+H21</f>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="2">
+        <f>G23+H23</f>
         <v>364.73</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>6.98</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>10.48</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>8.98</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <f>H23+SUM(H39:H42)</f>
+        <v>243.27000000000004</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G24:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>